<commit_message>
Fix: added promoter status for soft deletion of promoter
</commit_message>
<xml_diff>
--- a/api/resources/excel/Program/ProgramWorkbook.xlsx
+++ b/api/resources/excel/Program/ProgramWorkbook.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="36">
   <si>
     <t>program_summary_list</t>
   </si>
@@ -111,6 +111,15 @@
   </si>
   <si>
     <t>Affinity affiliate service</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>active, archived</t>
+  </si>
+  <si>
+    <t>archived</t>
   </si>
 </sst>
 </file>
@@ -856,31 +865,31 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="9">
-        <v>0.0</v>
-      </c>
+      <c r="A5" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="7"/>
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
+      <c r="I5" s="8" t="s">
+        <v>34</v>
+      </c>
       <c r="J5" s="7"/>
-      <c r="K5" s="9">
-        <v>91.0</v>
+      <c r="K5" s="8" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>13</v>
@@ -898,12 +907,12 @@
       <c r="I6" s="7"/>
       <c r="J6" s="7"/>
       <c r="K6" s="9">
-        <v>987.6</v>
+        <v>91.0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>13</v>
@@ -921,12 +930,12 @@
       <c r="I7" s="7"/>
       <c r="J7" s="7"/>
       <c r="K7" s="9">
-        <v>76.0</v>
+        <v>987.6</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>13</v>
@@ -944,12 +953,12 @@
       <c r="I8" s="7"/>
       <c r="J8" s="7"/>
       <c r="K8" s="9">
-        <v>18496.0</v>
+        <v>76.0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>13</v>
@@ -967,12 +976,12 @@
       <c r="I9" s="7"/>
       <c r="J9" s="7"/>
       <c r="K9" s="9">
-        <v>765.4</v>
+        <v>18496.0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>13</v>
@@ -990,6 +999,29 @@
       <c r="I10" s="7"/>
       <c r="J10" s="7"/>
       <c r="K10" s="9">
+        <v>765.4</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="9">
+        <v>0.0</v>
+      </c>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="9">
         <v>9127.0</v>
       </c>
     </row>

</xml_diff>